<commit_message>
new model for detection
</commit_message>
<xml_diff>
--- a/outputs/results/recording2/summary.xlsx
+++ b/outputs/results/recording2/summary.xlsx
@@ -480,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,7 +556,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0 0</t>
+          <t>test A</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -575,7 +575,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test A</t>
+          <t>test B .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -588,25 +588,6 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>test B .</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>